<commit_message>
main general formula calculate
</commit_message>
<xml_diff>
--- a/src/main/resources/RewardAmount2.xlsx
+++ b/src/main/resources/RewardAmount2.xlsx
@@ -85,7 +85,7 @@
     <t xml:space="preserve">petco</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;5</t>
+    <t xml:space="preserve">&lt;(6-1)</t>
   </si>
   <si>
     <t xml:space="preserve">REWARD_AMOUNT_TWO</t>
@@ -117,7 +117,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -175,12 +175,6 @@
       <name val="Tahoma"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -336,11 +330,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -348,7 +338,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -358,6 +348,10 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -437,13 +431,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.15"/>
@@ -575,83 +569,83 @@
         <v>14</v>
       </c>
       <c r="E9" s="12"/>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="12" t="s">
         <v>15</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="16" t="s">
+      <c r="E10" s="14"/>
+      <c r="F10" s="15" t="s">
         <v>19</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17" t="s">
+      <c r="B11" s="16"/>
+      <c r="C11" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="17" t="n">
+      <c r="D11" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="16" t="s">
         <v>23</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17" t="s">
+      <c r="B12" s="16"/>
+      <c r="C12" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="17" t="n">
+      <c r="D12" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="16" t="s">
         <v>26</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="17" t="n">
+      <c r="B13" s="16" t="n">
         <v>56787</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="18" t="s">
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="16" t="s">
         <v>28</v>
       </c>
       <c r="G13" s="6"/>
@@ -659,6 +653,9 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H14" s="6"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>